<commit_message>
Minor changes to DPoW to COBieLiteUK conversion, bug fixes in COBieLiteUK schema, more test cases for COBieLiteUK and XLS
</commit_message>
<xml_diff>
--- a/Xbim.COBieLiteUK/Templates/UK2012.xlsx
+++ b/Xbim.COBieLiteUK/Templates/UK2012.xlsx
@@ -35,7 +35,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">Connection!$A$1:$M$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Contact!$A$1:$S$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">Coordinate!$A$1:$O$88</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">Document!$A$1:$O$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">Document!$A$1:$O$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Facility!$A$1:$V$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Floor!$A$1:$J$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">Impact!$A$1:$P$29</definedName>
@@ -17796,7 +17796,7 @@
   <sheetPr>
     <tabColor indexed="42"/>
   </sheetPr>
-  <dimension ref="A1:O14"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -17865,43 +17865,34 @@
         <v>204</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="J9" s="10"/>
-    </row>
-    <row r="10" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="J10" s="10"/>
-    </row>
-    <row r="11" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="J11" s="10"/>
-    </row>
-    <row r="12" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="J12" s="10"/>
-    </row>
-    <row r="13" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="J13" s="10"/>
-    </row>
-    <row r="14" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="J14" s="10"/>
+    <row r="2" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="J2" s="10"/>
+    </row>
+    <row r="3" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="J3" s="10"/>
+    </row>
+    <row r="4" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="J4" s="10"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O8"/>
+  <autoFilter ref="A1:O1"/>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E9999">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E9989">
       <formula1>ApprovalBy</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L9999">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L9989">
       <formula1>objDocument</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D9999">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D9989">
       <formula1>DocumentType</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G9999">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G9989">
       <formula1>SheetType</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B9999">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B9989">
       <formula1>Contact.Name</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F9999">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F9989">
       <formula1>StageType</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
COBieLiteUK BS1192-4 validation implemented. It can also make the model compliant if it is possible (create default objects etc.)
</commit_message>
<xml_diff>
--- a/Xbim.COBieLiteUK/Templates/UK2012.xlsx
+++ b/Xbim.COBieLiteUK/Templates/UK2012.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="132" windowWidth="9996" windowHeight="9696" tabRatio="668" activeTab="7"/>
+    <workbookView xWindow="120" yWindow="132" windowWidth="9996" windowHeight="9696" tabRatio="668" firstSheet="5" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="Instruction" sheetId="21" r:id="rId1"/>
@@ -125,7 +125,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5317" uniqueCount="5063">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5317" uniqueCount="5064">
   <si>
     <t>Title</t>
   </si>
@@ -15314,6 +15314,9 @@
   </si>
   <si>
     <t>Uniclass G or RICS SFCA 2008</t>
+  </si>
+  <si>
+    <t>CostUnit</t>
   </si>
 </sst>
 </file>
@@ -18403,8 +18406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BC1965"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AU2" sqref="AU2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18573,7 +18576,7 @@
         <v>94</v>
       </c>
       <c r="AU1" s="7" t="s">
-        <v>95</v>
+        <v>5063</v>
       </c>
       <c r="AV1" s="7" t="s">
         <v>166</v>
@@ -37687,7 +37690,7 @@
   </sheetPr>
   <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>

<commit_message>
Performance improvements of COBieLiteUK
</commit_message>
<xml_diff>
--- a/Xbim.COBieLiteUK/Templates/UK2012.xlsx
+++ b/Xbim.COBieLiteUK/Templates/UK2012.xlsx
@@ -30766,7 +30766,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="40">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -30973,12 +30973,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFCC99FF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -31204,7 +31198,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -31228,7 +31222,6 @@
     <xf numFmtId="0" fontId="0" fillId="35" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="33" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -31239,8 +31232,7 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment textRotation="90"/>
@@ -31263,6 +31255,16 @@
     <xf numFmtId="0" fontId="0" fillId="35" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="33" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" textRotation="90" shrinkToFit="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -31621,19 +31623,17 @@
   </sheetPr>
   <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24.109375" customWidth="1"/>
     <col min="2" max="2" width="19.33203125" customWidth="1"/>
     <col min="3" max="3" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" style="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" style="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.109375" customWidth="1"/>
-    <col min="7" max="7" width="35.6640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.6640625" style="17" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="96.109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -31660,7 +31660,7 @@
       <c r="B3" s="2">
         <v>4</v>
       </c>
-      <c r="G3" s="22"/>
+      <c r="G3" s="21"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -31682,19 +31682,19 @@
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="19" t="s">
         <v>1957</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="20" t="s">
         <v>1958</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="E6" s="21" t="s">
         <v>1959</v>
       </c>
-      <c r="F6" s="23" t="s">
+      <c r="F6" s="22" t="s">
         <v>1960</v>
       </c>
-      <c r="G6" s="22" t="s">
+      <c r="G6" s="21" t="s">
         <v>1961</v>
       </c>
       <c r="H6" s="2" t="s">
@@ -31729,9 +31729,9 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C8" s="19"/>
+      <c r="C8" s="18"/>
       <c r="E8"/>
-      <c r="F8" s="18"/>
+      <c r="F8" s="17"/>
       <c r="G8"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -31741,19 +31741,19 @@
       <c r="B9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="19" t="s">
         <v>1957</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="20" t="s">
         <v>1958</v>
       </c>
-      <c r="E9" s="22" t="s">
+      <c r="E9" s="21" t="s">
         <v>1959</v>
       </c>
-      <c r="F9" s="23" t="s">
+      <c r="F9" s="22" t="s">
         <v>1960</v>
       </c>
-      <c r="G9" s="22" t="s">
+      <c r="G9" s="21" t="s">
         <v>1961</v>
       </c>
       <c r="H9" s="1" t="s">
@@ -31788,9 +31788,9 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C11" s="19"/>
+      <c r="C11" s="18"/>
       <c r="E11"/>
-      <c r="F11" s="18"/>
+      <c r="F11" s="17"/>
       <c r="G11"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -31800,19 +31800,19 @@
       <c r="B12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="19" t="s">
         <v>1957</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="20" t="s">
         <v>1958</v>
       </c>
-      <c r="E12" s="22" t="s">
+      <c r="E12" s="21" t="s">
         <v>1959</v>
       </c>
-      <c r="F12" s="23" t="s">
+      <c r="F12" s="22" t="s">
         <v>1960</v>
       </c>
-      <c r="G12" s="22" t="s">
+      <c r="G12" s="21" t="s">
         <v>1961</v>
       </c>
       <c r="H12" s="1" t="s">
@@ -31948,9 +31948,9 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C18" s="19"/>
+      <c r="C18" s="18"/>
       <c r="E18"/>
-      <c r="F18" s="18"/>
+      <c r="F18" s="17"/>
       <c r="G18"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -31960,19 +31960,19 @@
       <c r="B19" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="19" t="s">
         <v>1957</v>
       </c>
-      <c r="D19" s="21" t="s">
+      <c r="D19" s="20" t="s">
         <v>1958</v>
       </c>
-      <c r="E19" s="22" t="s">
+      <c r="E19" s="21" t="s">
         <v>1959</v>
       </c>
-      <c r="F19" s="23" t="s">
+      <c r="F19" s="22" t="s">
         <v>1960</v>
       </c>
-      <c r="G19" s="22" t="s">
+      <c r="G19" s="21" t="s">
         <v>1961</v>
       </c>
       <c r="H19" s="1" t="s">
@@ -32115,9 +32115,9 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C25" s="19"/>
+      <c r="C25" s="18"/>
       <c r="E25"/>
-      <c r="F25" s="18"/>
+      <c r="F25" s="17"/>
       <c r="G25"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -32127,19 +32127,19 @@
       <c r="B26" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C26" s="20" t="s">
+      <c r="C26" s="19" t="s">
         <v>1957</v>
       </c>
-      <c r="D26" s="21" t="s">
+      <c r="D26" s="20" t="s">
         <v>1958</v>
       </c>
-      <c r="E26" s="22" t="s">
+      <c r="E26" s="21" t="s">
         <v>1959</v>
       </c>
-      <c r="F26" s="23" t="s">
+      <c r="F26" s="22" t="s">
         <v>1960</v>
       </c>
-      <c r="G26" s="22" t="s">
+      <c r="G26" s="21" t="s">
         <v>1961</v>
       </c>
       <c r="H26" s="1" t="s">
@@ -32147,36 +32147,36 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C27" s="19"/>
+      <c r="C27" s="18"/>
       <c r="E27"/>
-      <c r="F27" s="18"/>
+      <c r="F27" s="17"/>
       <c r="G27"/>
       <c r="H27" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C28" s="19"/>
+      <c r="C28" s="18"/>
       <c r="E28"/>
-      <c r="F28" s="18"/>
+      <c r="F28" s="17"/>
       <c r="G28"/>
       <c r="H28" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C29" s="19"/>
+      <c r="C29" s="18"/>
       <c r="E29"/>
-      <c r="F29" s="18"/>
+      <c r="F29" s="17"/>
       <c r="G29"/>
       <c r="H29" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C30" s="19"/>
+      <c r="C30" s="18"/>
       <c r="E30"/>
-      <c r="F30" s="18"/>
+      <c r="F30" s="17"/>
       <c r="G30"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -32186,19 +32186,19 @@
       <c r="B31" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C31" s="20" t="s">
+      <c r="C31" s="19" t="s">
         <v>1957</v>
       </c>
-      <c r="D31" s="21" t="s">
+      <c r="D31" s="20" t="s">
         <v>1958</v>
       </c>
-      <c r="E31" s="22" t="s">
+      <c r="E31" s="21" t="s">
         <v>1959</v>
       </c>
-      <c r="F31" s="23" t="s">
+      <c r="F31" s="22" t="s">
         <v>1960</v>
       </c>
-      <c r="G31" s="22" t="s">
+      <c r="G31" s="21" t="s">
         <v>1961</v>
       </c>
       <c r="H31" s="1" t="s">
@@ -32287,47 +32287,47 @@
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C35" s="19"/>
+      <c r="C35" s="18"/>
       <c r="E35"/>
-      <c r="F35" s="18"/>
+      <c r="F35" s="17"/>
       <c r="G35"/>
       <c r="H35" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C36" s="19"/>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C36" s="18"/>
       <c r="E36"/>
-      <c r="F36" s="18"/>
+      <c r="F36" s="17"/>
       <c r="G36"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C37" s="20" t="s">
+      <c r="C37" s="19" t="s">
         <v>1957</v>
       </c>
-      <c r="D37" s="21" t="s">
+      <c r="D37" s="20" t="s">
         <v>1958</v>
       </c>
-      <c r="E37" s="22" t="s">
+      <c r="E37" s="21" t="s">
         <v>1959</v>
       </c>
-      <c r="F37" s="23" t="s">
+      <c r="F37" s="22" t="s">
         <v>1960</v>
       </c>
-      <c r="G37" s="22" t="s">
+      <c r="G37" s="21" t="s">
         <v>1961</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B38" s="3" t="s">
         <v>49</v>
       </c>
@@ -32354,7 +32354,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B39" s="3" t="s">
         <v>51</v>
       </c>
@@ -32381,7 +32381,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B40" s="3" t="s">
         <v>53</v>
       </c>
@@ -32408,7 +32408,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B41" s="3" t="s">
         <v>55</v>
       </c>
@@ -32517,13 +32517,13 @@
   <sheetPr>
     <tabColor indexed="42"/>
   </sheetPr>
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -32531,14 +32531,16 @@
     <col min="1" max="1" width="8.88671875" style="2" customWidth="1"/>
     <col min="2" max="2" width="8.88671875" style="4" customWidth="1"/>
     <col min="3" max="3" width="18.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="8.88671875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="28.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="30.77734375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="26.44140625" style="4" customWidth="1"/>
     <col min="7" max="7" width="8.88671875" style="4" customWidth="1"/>
     <col min="8" max="10" width="8.88671875" style="5" customWidth="1"/>
     <col min="11" max="11" width="21.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="21" width="8.88671875" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="74.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="30" customFormat="1" ht="73.8" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>88</v>
       </c>
@@ -32549,16 +32551,16 @@
         <v>72</v>
       </c>
       <c r="D1" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>159</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>162</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>110</v>
@@ -32572,6 +32574,16 @@
       <c r="K1" s="7" t="s">
         <v>102</v>
       </c>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:K7"/>
@@ -32598,13 +32610,13 @@
   <sheetPr>
     <tabColor indexed="42"/>
   </sheetPr>
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:AA1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -32618,9 +32630,10 @@
     <col min="10" max="10" width="7.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="11" max="13" width="8.88671875" style="5" customWidth="1"/>
     <col min="14" max="14" width="8.88671875" style="3" customWidth="1"/>
+    <col min="15" max="27" width="8.88671875" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="90.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" s="30" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>88</v>
       </c>
@@ -32663,6 +32676,19 @@
       <c r="N1" s="7" t="s">
         <v>102</v>
       </c>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="29"/>
+      <c r="W1" s="29"/>
+      <c r="X1" s="29"/>
+      <c r="Y1" s="29"/>
+      <c r="Z1" s="29"/>
+      <c r="AA1" s="29"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:M1"/>
@@ -32689,13 +32715,13 @@
   <sheetPr>
     <tabColor indexed="43"/>
   </sheetPr>
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:AE1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -32711,9 +32737,10 @@
     <col min="9" max="9" width="8.88671875" style="5" customWidth="1"/>
     <col min="10" max="10" width="29.5546875" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="8.88671875" style="3" customWidth="1"/>
+    <col min="13" max="31" width="8.88671875" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="63" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" s="30" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>88</v>
       </c>
@@ -32750,6 +32777,25 @@
       <c r="L1" s="7" t="s">
         <v>172</v>
       </c>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="29"/>
+      <c r="W1" s="29"/>
+      <c r="X1" s="29"/>
+      <c r="Y1" s="29"/>
+      <c r="Z1" s="29"/>
+      <c r="AA1" s="29"/>
+      <c r="AB1" s="29"/>
+      <c r="AC1" s="29"/>
+      <c r="AD1" s="29"/>
+      <c r="AE1" s="29"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:L8"/>
@@ -32776,13 +32822,13 @@
   <sheetPr>
     <tabColor indexed="43"/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -32793,9 +32839,10 @@
     <col min="4" max="4" width="8.88671875" style="4" customWidth="1"/>
     <col min="5" max="7" width="8.88671875" style="5" customWidth="1"/>
     <col min="8" max="8" width="22.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="17" width="8.88671875" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="30" customFormat="1" ht="61.8" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>88</v>
       </c>
@@ -32820,6 +32867,15 @@
       <c r="H1" s="7" t="s">
         <v>102</v>
       </c>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:H1"/>
@@ -32843,13 +32899,13 @@
   <sheetPr>
     <tabColor indexed="43"/>
   </sheetPr>
-  <dimension ref="A1:S13"/>
+  <dimension ref="A1:AE13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -32869,9 +32925,10 @@
     <col min="17" max="17" width="8.88671875" style="3" customWidth="1"/>
     <col min="18" max="18" width="8.88671875" style="4" customWidth="1"/>
     <col min="19" max="19" width="26.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="20" max="31" width="8.88671875" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="82.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" s="30" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>88</v>
       </c>
@@ -32929,43 +32986,55 @@
       <c r="S1" s="7" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="29"/>
+      <c r="W1" s="29"/>
+      <c r="X1" s="29"/>
+      <c r="Y1" s="29"/>
+      <c r="Z1" s="29"/>
+      <c r="AA1" s="29"/>
+      <c r="AB1" s="29"/>
+      <c r="AC1" s="29"/>
+      <c r="AD1" s="29"/>
+      <c r="AE1" s="29"/>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="J2" s="6"/>
     </row>
-    <row r="3" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="J3" s="6"/>
     </row>
-    <row r="4" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
       <c r="J4" s="6"/>
     </row>
-    <row r="5" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
       <c r="J5" s="6"/>
     </row>
-    <row r="6" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="J6" s="6"/>
     </row>
-    <row r="7" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
       <c r="J7" s="6"/>
     </row>
-    <row r="8" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
       <c r="J8" s="6"/>
     </row>
-    <row r="9" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
       <c r="J9" s="6"/>
     </row>
-    <row r="10" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
       <c r="J10" s="6"/>
     </row>
-    <row r="11" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
       <c r="J11" s="6"/>
     </row>
-    <row r="12" spans="1:19" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G12" s="25"/>
+    <row r="12" spans="1:31" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G12" s="24"/>
       <c r="J12" s="6"/>
     </row>
-    <row r="13" spans="1:19" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G13" s="25"/>
+    <row r="13" spans="1:31" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G13" s="24"/>
       <c r="J13" s="6"/>
     </row>
   </sheetData>
@@ -33005,13 +33074,13 @@
   <sheetPr>
     <tabColor indexed="42"/>
   </sheetPr>
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:AC1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33028,9 +33097,10 @@
     <col min="10" max="12" width="8.88671875" style="3" customWidth="1"/>
     <col min="13" max="15" width="8.88671875" style="5" customWidth="1"/>
     <col min="16" max="16" width="21.6640625" style="3" customWidth="1"/>
+    <col min="17" max="29" width="8.88671875" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="70.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" s="30" customFormat="1" ht="67.8" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>88</v>
       </c>
@@ -33079,6 +33149,19 @@
       <c r="P1" s="7" t="s">
         <v>102</v>
       </c>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="29"/>
+      <c r="W1" s="29"/>
+      <c r="X1" s="29"/>
+      <c r="Y1" s="29"/>
+      <c r="Z1" s="29"/>
+      <c r="AA1" s="29"/>
+      <c r="AB1" s="29"/>
+      <c r="AC1" s="29"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:P29">
@@ -33115,13 +33198,13 @@
   <sheetPr>
     <tabColor indexed="42"/>
   </sheetPr>
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:Y4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33135,9 +33218,10 @@
     <col min="10" max="10" width="104" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="13" width="8.88671875" style="5" customWidth="1"/>
     <col min="14" max="15" width="8.88671875" style="3" customWidth="1"/>
+    <col min="16" max="25" width="8.88671875" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="63" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" s="30" customFormat="1" ht="61.8" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>88</v>
       </c>
@@ -33183,14 +33267,24 @@
       <c r="O1" s="7" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="29"/>
+      <c r="W1" s="29"/>
+      <c r="X1" s="29"/>
+      <c r="Y1" s="29"/>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="J2" s="10"/>
     </row>
-    <row r="3" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="J3" s="10"/>
     </row>
-    <row r="4" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="J4" s="10"/>
     </row>
   </sheetData>
@@ -33224,13 +33318,13 @@
   <sheetPr>
     <tabColor indexed="42"/>
   </sheetPr>
-  <dimension ref="A1:AJ14"/>
+  <dimension ref="A1:AI14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33248,10 +33342,11 @@
     <col min="11" max="11" width="34.109375" style="5" customWidth="1"/>
     <col min="12" max="12" width="25.44140625" style="3" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.6640625" style="3" customWidth="1"/>
-    <col min="14" max="36" width="8.88671875" style="27" customWidth="1"/>
+    <col min="14" max="22" width="8.88671875" style="26" customWidth="1"/>
+    <col min="23" max="35" width="8.88671875" style="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="63" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" s="30" customFormat="1" ht="72.599999999999994" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>88</v>
       </c>
@@ -33288,48 +33383,57 @@
       <c r="L1" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="40" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="G2" s="24"/>
-    </row>
-    <row r="3" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="G3" s="24"/>
-    </row>
-    <row r="4" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="G4" s="24"/>
-    </row>
-    <row r="5" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="G5" s="24"/>
-    </row>
-    <row r="6" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="G6" s="24"/>
-    </row>
-    <row r="7" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="G7" s="24"/>
-    </row>
-    <row r="8" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="G8" s="24"/>
-    </row>
-    <row r="9" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="G9" s="24"/>
-    </row>
-    <row r="10" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="G10" s="24"/>
-    </row>
-    <row r="11" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="G11" s="24"/>
-    </row>
-    <row r="12" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="G12" s="24"/>
-    </row>
-    <row r="13" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="G13" s="24"/>
-    </row>
-    <row r="14" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="G14" s="24"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="29"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="G2" s="23"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="G3" s="23"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="G4" s="23"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="G5" s="23"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="G6" s="23"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="G7" s="23"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="G8" s="23"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="G9" s="23"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="G10" s="23"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="G11" s="23"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="G12" s="23"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="G13" s="23"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="G14" s="23"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:M16">
@@ -33364,13 +33468,13 @@
   <sheetPr>
     <tabColor indexed="42"/>
   </sheetPr>
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:W1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33382,9 +33486,10 @@
     <col min="7" max="9" width="9" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="12" width="8.88671875" style="5" customWidth="1"/>
     <col min="13" max="15" width="9" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="23" width="8.88671875" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" s="30" customFormat="1" ht="97.8" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>88</v>
       </c>
@@ -33430,6 +33535,14 @@
       <c r="O1" s="7" t="s">
         <v>210</v>
       </c>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="29"/>
+      <c r="W1" s="29"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:O88"/>
@@ -33456,13 +33569,13 @@
   <sheetPr>
     <tabColor indexed="42"/>
   </sheetPr>
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:Z1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33478,9 +33591,10 @@
     <col min="13" max="13" width="8.88671875" style="4" customWidth="1"/>
     <col min="14" max="14" width="8.88671875" style="2" customWidth="1"/>
     <col min="15" max="17" width="8.88671875" style="5" customWidth="1"/>
+    <col min="18" max="26" width="8.88671875" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="66" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" s="30" customFormat="1" ht="64.2" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>88</v>
       </c>
@@ -33532,6 +33646,15 @@
       <c r="Q1" s="7" t="s">
         <v>112</v>
       </c>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="29"/>
+      <c r="W1" s="29"/>
+      <c r="X1" s="29"/>
+      <c r="Y1" s="29"/>
+      <c r="Z1" s="29"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:Q1"/>
@@ -33589,10 +33712,10 @@
     <col min="11" max="11" width="8.88671875" style="3" customWidth="1"/>
     <col min="12" max="12" width="12.109375" style="3" bestFit="1" customWidth="1"/>
     <col min="13" max="19" width="8.88671875" style="3" customWidth="1"/>
-    <col min="20" max="40" width="8.88671875" style="28"/>
+    <col min="20" max="40" width="8.88671875" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" s="29" customFormat="1" ht="91.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:40" s="27" customFormat="1" ht="91.2" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>70</v>
       </c>
@@ -33650,27 +33773,27 @@
       <c r="S1" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="T1" s="30"/>
-      <c r="U1" s="30"/>
-      <c r="V1" s="30"/>
-      <c r="W1" s="30"/>
-      <c r="X1" s="30"/>
-      <c r="Y1" s="30"/>
-      <c r="Z1" s="30"/>
-      <c r="AA1" s="30"/>
-      <c r="AB1" s="30"/>
-      <c r="AC1" s="30"/>
-      <c r="AD1" s="30"/>
-      <c r="AE1" s="30"/>
-      <c r="AF1" s="30"/>
-      <c r="AG1" s="30"/>
-      <c r="AH1" s="30"/>
-      <c r="AI1" s="30"/>
-      <c r="AJ1" s="30"/>
-      <c r="AK1" s="30"/>
-      <c r="AL1" s="30"/>
-      <c r="AM1" s="30"/>
-      <c r="AN1" s="30"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
+      <c r="X1" s="28"/>
+      <c r="Y1" s="28"/>
+      <c r="Z1" s="28"/>
+      <c r="AA1" s="28"/>
+      <c r="AB1" s="28"/>
+      <c r="AC1" s="28"/>
+      <c r="AD1" s="28"/>
+      <c r="AE1" s="28"/>
+      <c r="AF1" s="28"/>
+      <c r="AG1" s="28"/>
+      <c r="AH1" s="28"/>
+      <c r="AI1" s="28"/>
+      <c r="AJ1" s="28"/>
+      <c r="AK1" s="28"/>
+      <c r="AL1" s="28"/>
+      <c r="AM1" s="28"/>
+      <c r="AN1" s="28"/>
     </row>
     <row r="2" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A2" s="10"/>
@@ -33741,10 +33864,10 @@
     <col min="32" max="32" width="10.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="43.109375" bestFit="1" customWidth="1"/>
-    <col min="35" max="46" width="8.88671875" style="28"/>
+    <col min="35" max="46" width="8.88671875" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" s="32" customFormat="1" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:46" s="30" customFormat="1" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>191</v>
       </c>
@@ -33844,21 +33967,21 @@
       <c r="AG1" s="7" t="s">
         <v>1901</v>
       </c>
-      <c r="AH1" s="36" t="s">
+      <c r="AH1" s="34" t="s">
         <v>1902</v>
       </c>
-      <c r="AI1" s="31"/>
-      <c r="AJ1" s="31"/>
-      <c r="AK1" s="31"/>
-      <c r="AL1" s="31"/>
-      <c r="AM1" s="31"/>
-      <c r="AN1" s="31"/>
-      <c r="AO1" s="31"/>
-      <c r="AP1" s="31"/>
-      <c r="AQ1" s="31"/>
-      <c r="AR1" s="31"/>
-      <c r="AS1" s="31"/>
-      <c r="AT1" s="31"/>
+      <c r="AI1" s="29"/>
+      <c r="AJ1" s="29"/>
+      <c r="AK1" s="29"/>
+      <c r="AL1" s="29"/>
+      <c r="AM1" s="29"/>
+      <c r="AN1" s="29"/>
+      <c r="AO1" s="29"/>
+      <c r="AP1" s="29"/>
+      <c r="AQ1" s="29"/>
+      <c r="AR1" s="29"/>
+      <c r="AS1" s="29"/>
+      <c r="AT1" s="29"/>
     </row>
     <row r="2" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -33960,7 +34083,7 @@
       <c r="AG2" s="2" t="s">
         <v>1903</v>
       </c>
-      <c r="AH2" s="37" t="s">
+      <c r="AH2" s="35" t="s">
         <v>1986</v>
       </c>
     </row>
@@ -34064,7 +34187,7 @@
       <c r="AG3" s="2" t="s">
         <v>1905</v>
       </c>
-      <c r="AH3" s="37" t="s">
+      <c r="AH3" s="35" t="s">
         <v>1987</v>
       </c>
     </row>
@@ -34162,7 +34285,7 @@
       <c r="AG4" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="AH4" s="37" t="s">
+      <c r="AH4" s="35" t="s">
         <v>1988</v>
       </c>
     </row>
@@ -34245,7 +34368,7 @@
       <c r="AG5" s="2" t="s">
         <v>1908</v>
       </c>
-      <c r="AH5" s="37" t="s">
+      <c r="AH5" s="35" t="s">
         <v>1989</v>
       </c>
     </row>
@@ -34322,7 +34445,7 @@
       <c r="AG6" s="2" t="s">
         <v>1919</v>
       </c>
-      <c r="AH6" s="37" t="s">
+      <c r="AH6" s="35" t="s">
         <v>1990</v>
       </c>
     </row>
@@ -34381,7 +34504,7 @@
       <c r="AG7" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="AH7" s="37" t="s">
+      <c r="AH7" s="35" t="s">
         <v>1991</v>
       </c>
     </row>
@@ -34428,7 +34551,7 @@
       <c r="AG8" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="AH8" s="37" t="s">
+      <c r="AH8" s="35" t="s">
         <v>1992</v>
       </c>
     </row>
@@ -34466,7 +34589,7 @@
       <c r="AG9" s="2" t="s">
         <v>1912</v>
       </c>
-      <c r="AH9" s="37" t="s">
+      <c r="AH9" s="35" t="s">
         <v>1993</v>
       </c>
     </row>
@@ -34504,7 +34627,7 @@
       <c r="AG10" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="AH10" s="37" t="s">
+      <c r="AH10" s="35" t="s">
         <v>1934</v>
       </c>
     </row>
@@ -34542,7 +34665,7 @@
       <c r="AG11" s="2" t="s">
         <v>1915</v>
       </c>
-      <c r="AH11" s="37" t="s">
+      <c r="AH11" s="35" t="s">
         <v>1936</v>
       </c>
     </row>
@@ -34577,7 +34700,7 @@
       <c r="AG12" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="AH12" s="37" t="s">
+      <c r="AH12" s="35" t="s">
         <v>1938</v>
       </c>
     </row>
@@ -34609,7 +34732,7 @@
       <c r="AG13" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="AH13" s="37" t="s">
+      <c r="AH13" s="35" t="s">
         <v>1939</v>
       </c>
     </row>
@@ -34641,7 +34764,7 @@
       <c r="AG14" s="2" t="s">
         <v>1921</v>
       </c>
-      <c r="AH14" s="37" t="s">
+      <c r="AH14" s="35" t="s">
         <v>1940</v>
       </c>
     </row>
@@ -34673,7 +34796,7 @@
       <c r="AG15" s="2" t="s">
         <v>1923</v>
       </c>
-      <c r="AH15" s="37" t="s">
+      <c r="AH15" s="35" t="s">
         <v>1941</v>
       </c>
     </row>
@@ -34705,7 +34828,7 @@
       <c r="AG16" s="2" t="s">
         <v>1925</v>
       </c>
-      <c r="AH16" s="37" t="s">
+      <c r="AH16" s="35" t="s">
         <v>1942</v>
       </c>
     </row>
@@ -34731,7 +34854,7 @@
       <c r="AG17" s="2" t="s">
         <v>1927</v>
       </c>
-      <c r="AH17" s="37" t="s">
+      <c r="AH17" s="35" t="s">
         <v>1943</v>
       </c>
     </row>
@@ -34757,7 +34880,7 @@
       <c r="AG18" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="AH18" s="37" t="s">
+      <c r="AH18" s="35" t="s">
         <v>1951</v>
       </c>
     </row>
@@ -34783,7 +34906,7 @@
       <c r="AG19" s="2" t="s">
         <v>1932</v>
       </c>
-      <c r="AH19" s="37" t="s">
+      <c r="AH19" s="35" t="s">
         <v>1945</v>
       </c>
     </row>
@@ -34809,7 +34932,7 @@
       <c r="AG20" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="AH20" s="37" t="s">
+      <c r="AH20" s="35" t="s">
         <v>1946</v>
       </c>
     </row>
@@ -34835,7 +34958,7 @@
       <c r="AG21" s="2" t="s">
         <v>1935</v>
       </c>
-      <c r="AH21" s="37" t="s">
+      <c r="AH21" s="35" t="s">
         <v>1947</v>
       </c>
     </row>
@@ -34861,7 +34984,7 @@
       <c r="AG22" s="2" t="s">
         <v>1937</v>
       </c>
-      <c r="AH22" s="37" t="s">
+      <c r="AH22" s="35" t="s">
         <v>1948</v>
       </c>
     </row>
@@ -34884,7 +35007,7 @@
       <c r="AG23" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="AH23" s="37" t="s">
+      <c r="AH23" s="35" t="s">
         <v>1949</v>
       </c>
     </row>
@@ -34907,7 +35030,7 @@
       <c r="AG24" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="AH24" s="37" t="s">
+      <c r="AH24" s="35" t="s">
         <v>1904</v>
       </c>
     </row>
@@ -34930,7 +35053,7 @@
       <c r="AG25" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="AH25" s="37" t="s">
+      <c r="AH25" s="35" t="s">
         <v>1906</v>
       </c>
     </row>
@@ -34953,7 +35076,7 @@
       <c r="AG26" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="AH26" s="37" t="s">
+      <c r="AH26" s="35" t="s">
         <v>1907</v>
       </c>
     </row>
@@ -34976,7 +35099,7 @@
       <c r="AG27" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="AH27" s="37" t="s">
+      <c r="AH27" s="35" t="s">
         <v>1909</v>
       </c>
     </row>
@@ -34999,7 +35122,7 @@
       <c r="AG28" s="2" t="s">
         <v>1944</v>
       </c>
-      <c r="AH28" s="37" t="s">
+      <c r="AH28" s="35" t="s">
         <v>1910</v>
       </c>
     </row>
@@ -35022,7 +35145,7 @@
       <c r="AG29" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="AH29" s="37" t="s">
+      <c r="AH29" s="35" t="s">
         <v>1911</v>
       </c>
     </row>
@@ -35045,7 +35168,7 @@
       <c r="AG30" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="AH30" s="37" t="s">
+      <c r="AH30" s="35" t="s">
         <v>1913</v>
       </c>
     </row>
@@ -35068,7 +35191,7 @@
       <c r="AG31" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="AH31" s="37" t="s">
+      <c r="AH31" s="35" t="s">
         <v>1914</v>
       </c>
     </row>
@@ -35091,7 +35214,7 @@
       <c r="AG32" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="AH32" s="37" t="s">
+      <c r="AH32" s="35" t="s">
         <v>1916</v>
       </c>
     </row>
@@ -35114,7 +35237,7 @@
       <c r="AG33" s="2" t="s">
         <v>1929</v>
       </c>
-      <c r="AH33" s="37" t="s">
+      <c r="AH33" s="35" t="s">
         <v>1917</v>
       </c>
     </row>
@@ -35137,7 +35260,7 @@
       <c r="AG34" s="2" t="s">
         <v>1950</v>
       </c>
-      <c r="AH34" s="37" t="s">
+      <c r="AH34" s="35" t="s">
         <v>1918</v>
       </c>
     </row>
@@ -35160,7 +35283,7 @@
       <c r="AG35" s="2" t="s">
         <v>1952</v>
       </c>
-      <c r="AH35" s="37" t="s">
+      <c r="AH35" s="35" t="s">
         <v>1920</v>
       </c>
     </row>
@@ -35183,7 +35306,7 @@
       <c r="AG36" s="2" t="s">
         <v>1953</v>
       </c>
-      <c r="AH36" s="37" t="s">
+      <c r="AH36" s="35" t="s">
         <v>1922</v>
       </c>
     </row>
@@ -35206,7 +35329,7 @@
       <c r="AG37" s="2" t="s">
         <v>1954</v>
       </c>
-      <c r="AH37" s="37" t="s">
+      <c r="AH37" s="35" t="s">
         <v>1924</v>
       </c>
     </row>
@@ -35229,7 +35352,7 @@
       <c r="AG38" s="2" t="s">
         <v>1955</v>
       </c>
-      <c r="AH38" s="37" t="s">
+      <c r="AH38" s="35" t="s">
         <v>1926</v>
       </c>
     </row>
@@ -35252,7 +35375,7 @@
       <c r="AG39" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="AH39" s="37" t="s">
+      <c r="AH39" s="35" t="s">
         <v>1928</v>
       </c>
     </row>
@@ -35272,7 +35395,7 @@
       <c r="H40" s="3" t="s">
         <v>407</v>
       </c>
-      <c r="AH40" s="37" t="s">
+      <c r="AH40" s="35" t="s">
         <v>1930</v>
       </c>
     </row>
@@ -35292,7 +35415,7 @@
       <c r="H41" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="AH41" s="37" t="s">
+      <c r="AH41" s="35" t="s">
         <v>1931</v>
       </c>
     </row>
@@ -35312,7 +35435,7 @@
       <c r="H42" s="3" t="s">
         <v>411</v>
       </c>
-      <c r="AH42" s="37" t="s">
+      <c r="AH42" s="35" t="s">
         <v>1933</v>
       </c>
     </row>
@@ -73658,50 +73781,50 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" style="33" customWidth="1"/>
-    <col min="2" max="2" width="16" style="34" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" style="33" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" style="34" customWidth="1"/>
-    <col min="5" max="5" width="23.5546875" style="28" customWidth="1"/>
-    <col min="6" max="8" width="8.88671875" style="35"/>
-    <col min="9" max="14" width="8.88671875" style="28"/>
+    <col min="1" max="1" width="18.33203125" style="31" customWidth="1"/>
+    <col min="2" max="2" width="16" style="32" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" style="31" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" style="32" customWidth="1"/>
+    <col min="5" max="5" width="23.5546875" style="26" customWidth="1"/>
+    <col min="6" max="8" width="8.88671875" style="33"/>
+    <col min="9" max="14" width="8.88671875" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="32" customFormat="1" ht="60.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:14" s="30" customFormat="1" ht="60.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="29" t="s">
         <v>110</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="H1" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="I1" s="31" t="s">
+      <c r="I1" s="29" t="s">
         <v>175</v>
       </c>
-      <c r="J1" s="31" t="s">
+      <c r="J1" s="29" t="s">
         <v>10158</v>
       </c>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -73735,10 +73858,10 @@
     <col min="12" max="18" width="8.88671875" style="5" customWidth="1"/>
     <col min="19" max="21" width="8.88671875" style="3" customWidth="1"/>
     <col min="22" max="22" width="43.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="38" width="8.88671875" style="28"/>
+    <col min="23" max="38" width="8.88671875" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" s="29" customFormat="1" ht="120.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:38" s="27" customFormat="1" ht="120.6" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>88</v>
       </c>
@@ -73805,22 +73928,22 @@
       <c r="V1" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="W1" s="30"/>
-      <c r="X1" s="30"/>
-      <c r="Y1" s="30"/>
-      <c r="Z1" s="30"/>
-      <c r="AA1" s="30"/>
-      <c r="AB1" s="30"/>
-      <c r="AC1" s="30"/>
-      <c r="AD1" s="30"/>
-      <c r="AE1" s="30"/>
-      <c r="AF1" s="30"/>
-      <c r="AG1" s="30"/>
-      <c r="AH1" s="30"/>
-      <c r="AI1" s="30"/>
-      <c r="AJ1" s="30"/>
-      <c r="AK1" s="30"/>
-      <c r="AL1" s="30"/>
+      <c r="W1" s="28"/>
+      <c r="X1" s="28"/>
+      <c r="Y1" s="28"/>
+      <c r="Z1" s="28"/>
+      <c r="AA1" s="28"/>
+      <c r="AB1" s="28"/>
+      <c r="AC1" s="28"/>
+      <c r="AD1" s="28"/>
+      <c r="AE1" s="28"/>
+      <c r="AF1" s="28"/>
+      <c r="AG1" s="28"/>
+      <c r="AH1" s="28"/>
+      <c r="AI1" s="28"/>
+      <c r="AJ1" s="28"/>
+      <c r="AK1" s="28"/>
+      <c r="AL1" s="28"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:V2"/>
@@ -73884,10 +74007,10 @@
     <col min="8" max="8" width="8.88671875" style="3" customWidth="1"/>
     <col min="9" max="9" width="9" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.88671875" style="3" customWidth="1"/>
-    <col min="11" max="21" width="8.88671875" style="28"/>
+    <col min="11" max="21" width="8.88671875" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="29" customFormat="1" ht="61.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" s="27" customFormat="1" ht="61.8" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>88</v>
       </c>
@@ -73918,17 +74041,17 @@
       <c r="J1" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="30"/>
-      <c r="S1" s="30"/>
-      <c r="T1" s="30"/>
-      <c r="U1" s="30"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J2"/>
@@ -73952,13 +74075,13 @@
   <sheetPr>
     <tabColor indexed="43"/>
   </sheetPr>
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -73973,9 +74096,10 @@
     <col min="8" max="9" width="8.88671875" style="5" customWidth="1"/>
     <col min="10" max="11" width="8.88671875" style="3" customWidth="1"/>
     <col min="12" max="13" width="9" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="23" width="8.88671875" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="69" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" s="38" customFormat="1" ht="67.8" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>88</v>
       </c>
@@ -74015,16 +74139,26 @@
       <c r="M1" s="7" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="37"/>
+      <c r="R1" s="37"/>
+      <c r="S1" s="37"/>
+      <c r="T1" s="37"/>
+      <c r="U1" s="37"/>
+      <c r="V1" s="37"/>
+      <c r="W1" s="37"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="L2" s="12"/>
       <c r="M2" s="12"/>
     </row>
-    <row r="3" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="L3" s="12"/>
       <c r="M3" s="12"/>
     </row>
-    <row r="4" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="L4" s="12"/>
       <c r="M4" s="12"/>
     </row>
@@ -74045,6 +74179,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -74053,13 +74188,13 @@
   <sheetPr>
     <tabColor indexed="42"/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:V1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -74071,9 +74206,10 @@
     <col min="5" max="5" width="19.5546875" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="8" width="8.88671875" style="5" customWidth="1"/>
     <col min="9" max="9" width="43.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="22" width="8.88671875" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" s="30" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>88</v>
       </c>
@@ -74101,6 +74237,19 @@
       <c r="I1" s="7" t="s">
         <v>102</v>
       </c>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="29"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:I1"/>
@@ -74164,10 +74313,10 @@
     <col min="25" max="29" width="8.88671875" style="3" customWidth="1"/>
     <col min="30" max="30" width="12.88671875" style="3" customWidth="1"/>
     <col min="31" max="35" width="8.88671875" style="3" customWidth="1"/>
-    <col min="36" max="46" width="8.88671875" style="28"/>
+    <col min="36" max="46" width="8.88671875" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" s="32" customFormat="1" ht="130.19999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:46" s="30" customFormat="1" ht="130.19999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>88</v>
       </c>
@@ -74273,17 +74422,17 @@
       <c r="AI1" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="AJ1" s="31"/>
-      <c r="AK1" s="31"/>
-      <c r="AL1" s="31"/>
-      <c r="AM1" s="31"/>
-      <c r="AN1" s="31"/>
-      <c r="AO1" s="31"/>
-      <c r="AP1" s="31"/>
-      <c r="AQ1" s="31"/>
-      <c r="AR1" s="31"/>
-      <c r="AS1" s="31"/>
-      <c r="AT1" s="31"/>
+      <c r="AJ1" s="29"/>
+      <c r="AK1" s="29"/>
+      <c r="AL1" s="29"/>
+      <c r="AM1" s="29"/>
+      <c r="AN1" s="29"/>
+      <c r="AO1" s="29"/>
+      <c r="AP1" s="29"/>
+      <c r="AQ1" s="29"/>
+      <c r="AR1" s="29"/>
+      <c r="AS1" s="29"/>
+      <c r="AT1" s="29"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AI15"/>
@@ -74339,10 +74488,10 @@
     <col min="13" max="13" width="9.33203125" style="16" customWidth="1"/>
     <col min="14" max="14" width="9.33203125" style="3" customWidth="1"/>
     <col min="15" max="15" width="8.88671875" style="3" customWidth="1"/>
-    <col min="16" max="26" width="8.88671875" style="28"/>
+    <col min="16" max="26" width="8.88671875" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="32" customFormat="1" ht="96" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" s="30" customFormat="1" ht="96" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>88</v>
       </c>
@@ -74388,17 +74537,17 @@
       <c r="O1" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="P1" s="38"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="31"/>
-      <c r="U1" s="31"/>
-      <c r="V1" s="31"/>
-      <c r="W1" s="31"/>
-      <c r="X1" s="31"/>
-      <c r="Y1" s="31"/>
-      <c r="Z1" s="31"/>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="29"/>
+      <c r="W1" s="29"/>
+      <c r="X1" s="29"/>
+      <c r="Y1" s="29"/>
+      <c r="Z1" s="29"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:O36"/>
@@ -74425,13 +74574,13 @@
   <sheetPr>
     <tabColor indexed="42"/>
   </sheetPr>
-  <dimension ref="A1:N36"/>
+  <dimension ref="A1:T36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -74443,11 +74592,11 @@
     <col min="5" max="5" width="39.44140625" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="8" width="8.88671875" style="5" customWidth="1"/>
     <col min="9" max="9" width="25.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.44140625" customWidth="1"/>
-    <col min="11" max="11" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.6640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="11" max="20" width="8.88671875" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="93.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" s="30" customFormat="1" ht="93" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>88</v>
       </c>
@@ -74475,245 +74624,122 @@
       <c r="I1" s="7" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-    </row>
-    <row r="3" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-    </row>
-    <row r="4" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="17"/>
-    </row>
-    <row r="5" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="J5" s="26"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
-    </row>
-    <row r="6" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="J6" s="26"/>
-      <c r="K6" s="26"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-    </row>
-    <row r="7" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="J7" s="26"/>
-      <c r="K7" s="26"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="17"/>
-    </row>
-    <row r="8" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="J8" s="26"/>
-      <c r="K8" s="26"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="17"/>
-      <c r="N8" s="17"/>
-    </row>
-    <row r="9" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="J9" s="26"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="17"/>
-      <c r="N9" s="17"/>
-    </row>
-    <row r="10" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="J10" s="26"/>
-      <c r="K10" s="26"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="17"/>
-    </row>
-    <row r="11" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="J11" s="26"/>
-      <c r="K11" s="26"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="17"/>
-    </row>
-    <row r="12" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="J12" s="26"/>
-      <c r="K12" s="26"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="17"/>
-      <c r="N12" s="17"/>
-    </row>
-    <row r="13" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="J13" s="26"/>
-      <c r="K13" s="26"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="17"/>
-      <c r="N13" s="17"/>
-    </row>
-    <row r="14" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="J14" s="26"/>
-      <c r="K14" s="26"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17"/>
-      <c r="N14" s="17"/>
-    </row>
-    <row r="15" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="J15" s="26"/>
-      <c r="K15" s="26"/>
-      <c r="L15" s="17"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="17"/>
-    </row>
-    <row r="16" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="J16" s="26"/>
-      <c r="K16" s="26"/>
-      <c r="L16" s="17"/>
-      <c r="M16" s="17"/>
-      <c r="N16" s="17"/>
-    </row>
-    <row r="17" spans="10:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="J17" s="26"/>
-      <c r="K17" s="26"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="17"/>
-      <c r="N17" s="17"/>
-    </row>
-    <row r="18" spans="10:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="J18" s="26"/>
-      <c r="K18" s="26"/>
-      <c r="L18" s="17"/>
-      <c r="M18" s="17"/>
-      <c r="N18" s="17"/>
-    </row>
-    <row r="19" spans="10:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="J19" s="26"/>
-      <c r="K19" s="26"/>
-      <c r="L19" s="17"/>
-      <c r="M19" s="17"/>
-      <c r="N19" s="17"/>
-    </row>
-    <row r="20" spans="10:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="J20" s="26"/>
-      <c r="K20" s="26"/>
-      <c r="L20" s="17"/>
-      <c r="M20" s="17"/>
-      <c r="N20" s="17"/>
-    </row>
-    <row r="21" spans="10:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="J21" s="26"/>
-      <c r="K21" s="26"/>
-      <c r="L21" s="17"/>
-      <c r="M21" s="17"/>
-      <c r="N21" s="17"/>
-    </row>
-    <row r="22" spans="10:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="J22" s="26"/>
-      <c r="K22" s="26"/>
-      <c r="L22" s="17"/>
-      <c r="M22" s="17"/>
-      <c r="N22" s="17"/>
-    </row>
-    <row r="23" spans="10:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="J23" s="26"/>
-      <c r="K23" s="26"/>
-      <c r="L23" s="17"/>
-      <c r="M23" s="17"/>
-      <c r="N23" s="17"/>
-    </row>
-    <row r="24" spans="10:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="J24" s="26"/>
-      <c r="K24" s="26"/>
-      <c r="L24" s="17"/>
-      <c r="M24" s="17"/>
-      <c r="N24" s="17"/>
-    </row>
-    <row r="25" spans="10:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="J25" s="26"/>
-      <c r="K25" s="26"/>
-      <c r="L25" s="17"/>
-      <c r="M25" s="17"/>
-      <c r="N25" s="17"/>
-    </row>
-    <row r="26" spans="10:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="J26" s="26"/>
-      <c r="K26" s="26"/>
-      <c r="L26" s="17"/>
-      <c r="M26" s="17"/>
-      <c r="N26" s="17"/>
-    </row>
-    <row r="27" spans="10:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="J27" s="26"/>
-      <c r="K27" s="26"/>
-      <c r="L27" s="17"/>
-      <c r="M27" s="17"/>
-      <c r="N27" s="17"/>
-    </row>
-    <row r="28" spans="10:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="J28" s="26"/>
-      <c r="K28" s="26"/>
-      <c r="L28" s="17"/>
-      <c r="M28" s="17"/>
-      <c r="N28" s="17"/>
-    </row>
-    <row r="29" spans="10:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="J29" s="26"/>
-      <c r="K29" s="26"/>
-      <c r="L29" s="17"/>
-      <c r="M29" s="17"/>
-      <c r="N29" s="17"/>
-    </row>
-    <row r="30" spans="10:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="J30" s="26"/>
-      <c r="K30" s="26"/>
-      <c r="L30" s="17"/>
-      <c r="M30" s="17"/>
-      <c r="N30" s="17"/>
-    </row>
-    <row r="31" spans="10:14" x14ac:dyDescent="0.3">
-      <c r="J31" s="26"/>
-      <c r="K31" s="26"/>
-      <c r="L31" s="17"/>
-      <c r="M31" s="17"/>
-      <c r="N31" s="17"/>
-    </row>
-    <row r="32" spans="10:14" x14ac:dyDescent="0.3">
-      <c r="J32" s="26"/>
-      <c r="K32" s="26"/>
-      <c r="L32" s="17"/>
-      <c r="M32" s="17"/>
-      <c r="N32" s="17"/>
-    </row>
-    <row r="33" spans="10:14" x14ac:dyDescent="0.3">
-      <c r="J33" s="26"/>
-      <c r="K33" s="26"/>
-      <c r="L33" s="17"/>
-      <c r="M33" s="17"/>
-      <c r="N33" s="17"/>
-    </row>
-    <row r="34" spans="10:14" x14ac:dyDescent="0.3">
-      <c r="J34" s="26"/>
-      <c r="K34" s="26"/>
-      <c r="L34" s="17"/>
-      <c r="M34" s="17"/>
-      <c r="N34" s="17"/>
-    </row>
-    <row r="35" spans="10:14" x14ac:dyDescent="0.3">
-      <c r="J35" s="26"/>
-      <c r="K35" s="26"/>
-      <c r="L35" s="17"/>
-      <c r="M35" s="17"/>
-      <c r="N35" s="17"/>
-    </row>
-    <row r="36" spans="10:14" x14ac:dyDescent="0.3">
-      <c r="J36" s="26"/>
-      <c r="K36" s="26"/>
-      <c r="L36" s="17"/>
-      <c r="M36" s="17"/>
-      <c r="N36" s="17"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="J2" s="39"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="J3" s="39"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="J4" s="39"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="J5" s="39"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="J6" s="39"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="J7" s="39"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="J8" s="39"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="J9" s="39"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="J10" s="39"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="J11" s="39"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="J12" s="39"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="J13" s="39"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="J14" s="39"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="J15" s="39"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="J16" s="39"/>
+    </row>
+    <row r="17" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J17" s="39"/>
+    </row>
+    <row r="18" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J18" s="39"/>
+    </row>
+    <row r="19" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J19" s="39"/>
+    </row>
+    <row r="20" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J20" s="39"/>
+    </row>
+    <row r="21" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J21" s="39"/>
+    </row>
+    <row r="22" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J22" s="39"/>
+    </row>
+    <row r="23" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J23" s="39"/>
+    </row>
+    <row r="24" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J24" s="39"/>
+    </row>
+    <row r="25" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J25" s="39"/>
+    </row>
+    <row r="26" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J26" s="39"/>
+    </row>
+    <row r="27" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J27" s="39"/>
+    </row>
+    <row r="28" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J28" s="39"/>
+    </row>
+    <row r="29" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J29" s="39"/>
+    </row>
+    <row r="30" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J30" s="39"/>
+    </row>
+    <row r="31" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J31" s="39"/>
+    </row>
+    <row r="32" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J32" s="39"/>
+    </row>
+    <row r="33" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J33" s="39"/>
+    </row>
+    <row r="34" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J34" s="39"/>
+    </row>
+    <row r="35" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J35" s="39"/>
+    </row>
+    <row r="36" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J36" s="39"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:I5"/>
@@ -74724,7 +74750,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E9999">
       <formula1>Component.Name</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:K36 D2:D9999">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D9999 J2:J36">
       <formula1>Table21</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B9999">

</xml_diff>